<commit_message>
Add stop propagation in modalTest
</commit_message>
<xml_diff>
--- a/vue_scheme.xlsx
+++ b/vue_scheme.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\test\a\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{668560DF-4830-4B10-9EF0-994B647D259A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5A78DD-2602-4B54-A3BC-021AF0EDB000}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6510" yWindow="0" windowWidth="8280" windowHeight="7520" xr2:uid="{36048C15-E544-4B43-B34D-766EA946C971}"/>
+    <workbookView xWindow="7440" yWindow="0" windowWidth="8280" windowHeight="7520" xr2:uid="{36048C15-E544-4B43-B34D-766EA946C971}"/>
   </bookViews>
   <sheets>
     <sheet name="admin_dev" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="367">
   <si>
     <t>theme.js</t>
   </si>
@@ -1106,9 +1106,6 @@
     <t>$emit('ok')</t>
   </si>
   <si>
-    <t>$emit('close')</t>
-  </si>
-  <si>
     <t>@ok</t>
   </si>
   <si>
@@ -1128,6 +1125,9 @@
   </si>
   <si>
     <t>handleClose() {this.isPopOpen = false}</t>
+  </si>
+  <si>
+    <t>close(){this.$emit('close')}</t>
   </si>
 </sst>
 </file>
@@ -1362,7 +1362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1457,25 +1457,17 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1484,10 +1476,10 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1502,14 +1494,26 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1519,12 +1523,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1955,7 +1953,7 @@
   <dimension ref="A1:AK55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="X1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="AF3" sqref="AF3"/>
+      <selection activeCell="AD7" sqref="AD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1976,42 +1974,42 @@
       <c r="D1" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="G1" s="85" t="s">
+      <c r="G1" s="81" t="s">
         <v>261</v>
       </c>
-      <c r="H1" s="86"/>
+      <c r="H1" s="82"/>
       <c r="I1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="85" t="s">
+      <c r="J1" s="81" t="s">
         <v>266</v>
       </c>
-      <c r="K1" s="86"/>
-      <c r="M1" s="85" t="s">
+      <c r="K1" s="82"/>
+      <c r="M1" s="81" t="s">
         <v>264</v>
       </c>
-      <c r="N1" s="86"/>
+      <c r="N1" s="82"/>
       <c r="O1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="85" t="s">
+      <c r="P1" s="81" t="s">
         <v>265</v>
       </c>
-      <c r="Q1" s="86"/>
+      <c r="Q1" s="82"/>
       <c r="R1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="85" t="s">
+      <c r="S1" s="81" t="s">
         <v>263</v>
       </c>
-      <c r="T1" s="86"/>
+      <c r="T1" s="82"/>
       <c r="U1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="V1" s="85" t="s">
+      <c r="V1" s="81" t="s">
         <v>267</v>
       </c>
-      <c r="W1" s="86"/>
+      <c r="W1" s="82"/>
       <c r="X1" s="15" t="s">
         <v>2</v>
       </c>
@@ -2165,7 +2163,7 @@
         <v>2</v>
       </c>
       <c r="Y3" s="77" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="Z3" s="78"/>
       <c r="AA3" s="15" t="s">
@@ -2239,7 +2237,7 @@
         <v>2</v>
       </c>
       <c r="AB4" s="65" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="AC4" s="79" t="s">
         <v>358</v>
@@ -2289,20 +2287,18 @@
         <v>2</v>
       </c>
       <c r="Y5" s="52" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="Z5" s="53" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AA5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="AB5" s="80" t="s">
-        <v>364</v>
-      </c>
-      <c r="AC5" s="81" t="s">
-        <v>359</v>
-      </c>
+      <c r="AB5" s="65" t="s">
+        <v>363</v>
+      </c>
+      <c r="AC5" s="79"/>
       <c r="AD5" s="15" t="s">
         <v>2</v>
       </c>
@@ -2327,13 +2323,19 @@
         <v>2</v>
       </c>
       <c r="Y6" s="43" t="s">
-        <v>361</v>
-      </c>
-      <c r="Z6" s="82" t="s">
+        <v>360</v>
+      </c>
+      <c r="Z6" s="80" t="s">
+        <v>365</v>
+      </c>
+      <c r="AA6" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB6" s="43" t="s">
+        <v>159</v>
+      </c>
+      <c r="AC6" s="44" t="s">
         <v>366</v>
-      </c>
-      <c r="AA6" s="15" t="s">
-        <v>2</v>
       </c>
       <c r="AD6" s="15" t="s">
         <v>2</v>
@@ -2437,17 +2439,17 @@
       </c>
     </row>
     <row r="11" spans="1:34" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="93" t="s">
+      <c r="A11" s="89" t="s">
         <v>274</v>
       </c>
-      <c r="B11" s="94"/>
+      <c r="B11" s="90"/>
       <c r="C11" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="85" t="s">
+      <c r="D11" s="81" t="s">
         <v>274</v>
       </c>
-      <c r="E11" s="86"/>
+      <c r="E11" s="82"/>
       <c r="F11" s="15" t="s">
         <v>2</v>
       </c>
@@ -2477,31 +2479,31 @@
       <c r="C12" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="89" t="s">
+      <c r="D12" s="85" t="s">
         <v>230</v>
       </c>
-      <c r="E12" s="90"/>
+      <c r="E12" s="86"/>
       <c r="F12" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G12" s="85" t="s">
+      <c r="G12" s="81" t="s">
         <v>277</v>
       </c>
-      <c r="H12" s="86"/>
+      <c r="H12" s="82"/>
       <c r="I12" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="J12" s="85" t="s">
+      <c r="J12" s="81" t="s">
         <v>162</v>
       </c>
-      <c r="K12" s="86"/>
+      <c r="K12" s="82"/>
       <c r="L12" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="V12" s="85" t="s">
+      <c r="V12" s="81" t="s">
         <v>306</v>
       </c>
-      <c r="W12" s="86"/>
+      <c r="W12" s="82"/>
       <c r="X12" s="45" t="s">
         <v>2</v>
       </c>
@@ -2549,10 +2551,10 @@
       <c r="L13" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="M13" s="85" t="s">
+      <c r="M13" s="81" t="s">
         <v>181</v>
       </c>
-      <c r="N13" s="86"/>
+      <c r="N13" s="82"/>
       <c r="O13" s="15" t="s">
         <v>2</v>
       </c>
@@ -2568,10 +2570,10 @@
       <c r="X13" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="Y13" s="85" t="s">
+      <c r="Y13" s="81" t="s">
         <v>309</v>
       </c>
-      <c r="Z13" s="86"/>
+      <c r="Z13" s="82"/>
       <c r="AA13" s="15" t="s">
         <v>2</v>
       </c>
@@ -2586,10 +2588,10 @@
       </c>
     </row>
     <row r="14" spans="1:34" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="85" t="s">
+      <c r="A14" s="81" t="s">
         <v>164</v>
       </c>
-      <c r="B14" s="86"/>
+      <c r="B14" s="82"/>
       <c r="C14" s="15" t="s">
         <v>2</v>
       </c>
@@ -2627,10 +2629,10 @@
       <c r="O14" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="P14" s="85" t="s">
+      <c r="P14" s="81" t="s">
         <v>197</v>
       </c>
-      <c r="Q14" s="86"/>
+      <c r="Q14" s="82"/>
       <c r="R14" s="15" t="s">
         <v>2</v>
       </c>
@@ -2655,10 +2657,10 @@
       <c r="AA14" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="AB14" s="85" t="s">
+      <c r="AB14" s="81" t="s">
         <v>318</v>
       </c>
-      <c r="AC14" s="86"/>
+      <c r="AC14" s="82"/>
       <c r="AD14" s="15" t="s">
         <v>2</v>
       </c>
@@ -2677,10 +2679,10 @@
       <c r="C15" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="89" t="s">
+      <c r="D15" s="85" t="s">
         <v>287</v>
       </c>
-      <c r="E15" s="90"/>
+      <c r="E15" s="86"/>
       <c r="F15" s="15" t="s">
         <v>2</v>
       </c>
@@ -2691,10 +2693,10 @@
       <c r="I15" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="J15" s="89" t="s">
+      <c r="J15" s="85" t="s">
         <v>195</v>
       </c>
-      <c r="K15" s="90"/>
+      <c r="K15" s="86"/>
       <c r="L15" s="15" t="s">
         <v>2</v>
       </c>
@@ -2719,10 +2721,10 @@
       <c r="U15" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="V15" s="89" t="s">
+      <c r="V15" s="85" t="s">
         <v>195</v>
       </c>
-      <c r="W15" s="90"/>
+      <c r="W15" s="86"/>
       <c r="X15" s="45" t="s">
         <v>2</v>
       </c>
@@ -2742,10 +2744,10 @@
       <c r="AD15" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="AE15" s="85" t="s">
+      <c r="AE15" s="81" t="s">
         <v>343</v>
       </c>
-      <c r="AF15" s="86"/>
+      <c r="AF15" s="82"/>
       <c r="AG15" s="15" t="s">
         <v>2</v>
       </c>
@@ -3055,10 +3057,10 @@
       <c r="C19" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="89" t="s">
+      <c r="D19" s="85" t="s">
         <v>288</v>
       </c>
-      <c r="E19" s="90"/>
+      <c r="E19" s="86"/>
       <c r="F19" s="15" t="s">
         <v>2</v>
       </c>
@@ -3137,10 +3139,10 @@
       </c>
     </row>
     <row r="20" spans="1:37" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="95" t="s">
+      <c r="A20" s="91" t="s">
         <v>176</v>
       </c>
-      <c r="B20" s="96"/>
+      <c r="B20" s="92"/>
       <c r="C20" s="15" t="s">
         <v>2</v>
       </c>
@@ -3153,10 +3155,10 @@
       <c r="F20" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G20" s="89" t="s">
+      <c r="G20" s="85" t="s">
         <v>230</v>
       </c>
-      <c r="H20" s="90"/>
+      <c r="H20" s="86"/>
       <c r="I20" s="15" t="s">
         <v>2</v>
       </c>
@@ -3235,10 +3237,10 @@
       <c r="C21" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="89" t="s">
+      <c r="D21" s="85" t="s">
         <v>289</v>
       </c>
-      <c r="E21" s="90"/>
+      <c r="E21" s="86"/>
       <c r="F21" s="15" t="s">
         <v>2</v>
       </c>
@@ -3378,10 +3380,10 @@
       <c r="U22" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="V22" s="91" t="s">
+      <c r="V22" s="93" t="s">
         <v>309</v>
       </c>
-      <c r="W22" s="92"/>
+      <c r="W22" s="94"/>
       <c r="X22" s="45" t="s">
         <v>2</v>
       </c>
@@ -3425,24 +3427,24 @@
       <c r="C23" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="89" t="s">
+      <c r="D23" s="85" t="s">
         <v>290</v>
       </c>
-      <c r="E23" s="90"/>
+      <c r="E23" s="86"/>
       <c r="F23" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G23" s="89" t="s">
+      <c r="G23" s="85" t="s">
         <v>280</v>
       </c>
-      <c r="H23" s="90"/>
+      <c r="H23" s="86"/>
       <c r="I23" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="J23" s="91" t="s">
+      <c r="J23" s="93" t="s">
         <v>181</v>
       </c>
-      <c r="K23" s="92"/>
+      <c r="K23" s="94"/>
       <c r="L23" s="15" t="s">
         <v>2</v>
       </c>
@@ -3494,10 +3496,10 @@
       <c r="AD23" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="AE23" s="89" t="s">
+      <c r="AE23" s="85" t="s">
         <v>230</v>
       </c>
-      <c r="AF23" s="90"/>
+      <c r="AF23" s="86"/>
       <c r="AG23" s="15" t="s">
         <v>2</v>
       </c>
@@ -3554,10 +3556,10 @@
       <c r="O24" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="P24" s="89" t="s">
+      <c r="P24" s="85" t="s">
         <v>230</v>
       </c>
-      <c r="Q24" s="90"/>
+      <c r="Q24" s="86"/>
       <c r="R24" s="15" t="s">
         <v>2</v>
       </c>
@@ -3612,10 +3614,10 @@
       <c r="F25" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G25" s="89" t="s">
+      <c r="G25" s="85" t="s">
         <v>285</v>
       </c>
-      <c r="H25" s="90"/>
+      <c r="H25" s="86"/>
       <c r="I25" s="15" t="s">
         <v>2</v>
       </c>
@@ -3749,10 +3751,10 @@
       <c r="AD26" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="AE26" s="89" t="s">
+      <c r="AE26" s="85" t="s">
         <v>340</v>
       </c>
-      <c r="AF26" s="90"/>
+      <c r="AF26" s="86"/>
       <c r="AG26" s="15" t="s">
         <v>2</v>
       </c>
@@ -3764,10 +3766,10 @@
       </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A27" s="85" t="s">
+      <c r="A27" s="81" t="s">
         <v>199</v>
       </c>
-      <c r="B27" s="86"/>
+      <c r="B27" s="82"/>
       <c r="C27" s="15" t="s">
         <v>2</v>
       </c>
@@ -3778,10 +3780,10 @@
       <c r="F27" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G27" s="89" t="s">
+      <c r="G27" s="85" t="s">
         <v>286</v>
       </c>
-      <c r="H27" s="90"/>
+      <c r="H27" s="86"/>
       <c r="I27" s="15" t="s">
         <v>2</v>
       </c>
@@ -3797,10 +3799,10 @@
       <c r="O27" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="P27" s="89" t="s">
+      <c r="P27" s="85" t="s">
         <v>231</v>
       </c>
-      <c r="Q27" s="90"/>
+      <c r="Q27" s="86"/>
       <c r="U27" s="15" t="s">
         <v>2</v>
       </c>
@@ -3934,10 +3936,10 @@
       <c r="C29" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="93" t="s">
+      <c r="D29" s="89" t="s">
         <v>163</v>
       </c>
-      <c r="E29" s="94"/>
+      <c r="E29" s="90"/>
       <c r="F29" s="15" t="s">
         <v>2</v>
       </c>
@@ -4027,10 +4029,10 @@
       <c r="O30" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="P30" s="89" t="s">
+      <c r="P30" s="85" t="s">
         <v>232</v>
       </c>
-      <c r="Q30" s="90"/>
+      <c r="Q30" s="86"/>
       <c r="R30" s="15" t="s">
         <v>2</v>
       </c>
@@ -4167,10 +4169,10 @@
       <c r="O32" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="P32" s="89" t="s">
+      <c r="P32" s="85" t="s">
         <v>233</v>
       </c>
-      <c r="Q32" s="90"/>
+      <c r="Q32" s="86"/>
       <c r="R32" s="15" t="s">
         <v>2</v>
       </c>
@@ -4518,10 +4520,10 @@
       </c>
     </row>
     <row r="39" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A39" s="89" t="s">
+      <c r="A39" s="85" t="s">
         <v>218</v>
       </c>
-      <c r="B39" s="90"/>
+      <c r="B39" s="86"/>
       <c r="C39" s="15" t="s">
         <v>2</v>
       </c>
@@ -4551,10 +4553,10 @@
       </c>
     </row>
     <row r="40" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A40" s="89" t="s">
+      <c r="A40" s="85" t="s">
         <v>219</v>
       </c>
-      <c r="B40" s="90"/>
+      <c r="B40" s="86"/>
       <c r="C40" s="15" t="s">
         <v>2</v>
       </c>
@@ -4584,10 +4586,10 @@
       </c>
     </row>
     <row r="41" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A41" s="89" t="s">
+      <c r="A41" s="85" t="s">
         <v>224</v>
       </c>
-      <c r="B41" s="90"/>
+      <c r="B41" s="86"/>
       <c r="C41" s="15" t="s">
         <v>2</v>
       </c>
@@ -4763,15 +4765,55 @@
     </row>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="Y30:Z30"/>
+    <mergeCell ref="Y34:Z34"/>
+    <mergeCell ref="AE15:AF15"/>
+    <mergeCell ref="AE18:AF18"/>
+    <mergeCell ref="AB25:AC25"/>
+    <mergeCell ref="AB27:AC27"/>
+    <mergeCell ref="AE28:AF28"/>
+    <mergeCell ref="AE23:AF23"/>
+    <mergeCell ref="AE26:AF26"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="V15:W15"/>
+    <mergeCell ref="Y22:Z22"/>
+    <mergeCell ref="Y26:Z26"/>
+    <mergeCell ref="Y13:Z13"/>
+    <mergeCell ref="Y15:Z15"/>
+    <mergeCell ref="V20:W20"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="V12:W12"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D11:E11"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="P14:Q14"/>
@@ -4788,59 +4830,19 @@
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="P4:Q4"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="S1:T1"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="S4:T4"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="V12:W12"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="AB14:AC14"/>
-    <mergeCell ref="V15:W15"/>
-    <mergeCell ref="Y22:Z22"/>
-    <mergeCell ref="Y26:Z26"/>
-    <mergeCell ref="Y13:Z13"/>
-    <mergeCell ref="Y15:Z15"/>
-    <mergeCell ref="V20:W20"/>
-    <mergeCell ref="V22:W22"/>
-    <mergeCell ref="Y30:Z30"/>
-    <mergeCell ref="Y34:Z34"/>
-    <mergeCell ref="AE15:AF15"/>
-    <mergeCell ref="AE18:AF18"/>
-    <mergeCell ref="AB25:AC25"/>
-    <mergeCell ref="AB27:AC27"/>
-    <mergeCell ref="AE28:AF28"/>
-    <mergeCell ref="AE23:AF23"/>
-    <mergeCell ref="AE26:AF26"/>
-    <mergeCell ref="AB16:AC16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -4983,7 +4985,7 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="98"/>
+      <c r="A4" s="96"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
@@ -5010,7 +5012,7 @@
       <c r="O4" s="2"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A5" s="99" t="s">
+      <c r="A5" s="95" t="s">
         <v>89</v>
       </c>
       <c r="B5" s="5"/>
@@ -5038,7 +5040,7 @@
       <c r="O5" s="5"/>
     </row>
     <row r="6" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="98"/>
+      <c r="A6" s="96"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
@@ -5154,7 +5156,7 @@
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A10" s="99" t="s">
+      <c r="A10" s="95" t="s">
         <v>94</v>
       </c>
       <c r="B10" s="5"/>
@@ -5200,7 +5202,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="98"/>
+      <c r="A11" s="96"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="19" t="s">
@@ -5299,7 +5301,7 @@
       <c r="O14" s="12"/>
     </row>
     <row r="15" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="98"/>
+      <c r="A15" s="96"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
@@ -5353,10 +5355,10 @@
       <c r="O16" s="12"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A17" s="99" t="s">
+      <c r="A17" s="95" t="s">
         <v>112</v>
       </c>
-      <c r="B17" s="103" t="s">
+      <c r="B17" s="98" t="s">
         <v>133</v>
       </c>
       <c r="C17" s="5"/>
@@ -5379,7 +5381,7 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="97"/>
-      <c r="B18" s="104"/>
+      <c r="B18" s="99"/>
       <c r="C18" s="1"/>
       <c r="D18" s="3" t="s">
         <v>13</v>
@@ -5400,7 +5402,7 @@
     </row>
     <row r="19" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="97"/>
-      <c r="B19" s="98"/>
+      <c r="B19" s="96"/>
       <c r="C19" s="2"/>
       <c r="D19" s="18" t="s">
         <v>14</v>
@@ -5421,7 +5423,7 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="97"/>
-      <c r="B20" s="99" t="s">
+      <c r="B20" s="95" t="s">
         <v>10</v>
       </c>
       <c r="C20" s="5"/>
@@ -5465,7 +5467,7 @@
     </row>
     <row r="22" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="97"/>
-      <c r="B22" s="98"/>
+      <c r="B22" s="96"/>
       <c r="C22" s="2"/>
       <c r="D22" s="18" t="s">
         <v>130</v>
@@ -5486,7 +5488,7 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="97"/>
-      <c r="B23" s="99" t="s">
+      <c r="B23" s="95" t="s">
         <v>3</v>
       </c>
       <c r="C23" s="5"/>
@@ -5509,7 +5511,7 @@
     </row>
     <row r="24" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="97"/>
-      <c r="B24" s="98"/>
+      <c r="B24" s="96"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
         <v>0</v>
@@ -5542,7 +5544,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="97"/>
-      <c r="B25" s="99" t="s">
+      <c r="B25" s="95" t="s">
         <v>11</v>
       </c>
       <c r="C25" s="5"/>
@@ -5565,7 +5567,7 @@
     </row>
     <row r="26" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="97"/>
-      <c r="B26" s="98"/>
+      <c r="B26" s="96"/>
       <c r="C26" s="2"/>
       <c r="D26" s="18" t="s">
         <v>126</v>
@@ -5676,7 +5678,7 @@
       <c r="O29" s="1"/>
     </row>
     <row r="30" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="98"/>
+      <c r="A30" s="96"/>
       <c r="B30" s="18" t="s">
         <v>35</v>
       </c>
@@ -5758,7 +5760,7 @@
       <c r="O33" s="1"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A34" s="99" t="s">
+      <c r="A34" s="95" t="s">
         <v>138</v>
       </c>
       <c r="B34" s="5"/>
@@ -5780,7 +5782,7 @@
       <c r="O34" s="5"/>
     </row>
     <row r="35" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="98"/>
+      <c r="A35" s="96"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
@@ -5945,11 +5947,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="A17:A30"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A34:A35"/>
     <mergeCell ref="A5:A6"/>
@@ -5957,6 +5954,11 @@
     <mergeCell ref="A12:A15"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="A17:A30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add setLocale function in el-menu
</commit_message>
<xml_diff>
--- a/vue_scheme.xlsx
+++ b/vue_scheme.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\test\a\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED7269F9-C22E-4BA9-A2D3-6DC677E622D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98FB2E45-31B5-4144-A50F-8F3F57515254}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10230" yWindow="0" windowWidth="8280" windowHeight="7520" xr2:uid="{36048C15-E544-4B43-B34D-766EA946C971}"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="8280" windowHeight="1520" firstSheet="1" activeTab="4" xr2:uid="{36048C15-E544-4B43-B34D-766EA946C971}"/>
   </bookViews>
   <sheets>
     <sheet name="admin_dev" sheetId="2" r:id="rId1"/>
     <sheet name="components" sheetId="3" r:id="rId2"/>
     <sheet name="editor_bundle" sheetId="1" r:id="rId3"/>
+    <sheet name="ninja" sheetId="4" r:id="rId4"/>
+    <sheet name="translate" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1539" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1738" uniqueCount="466">
   <si>
     <t>theme.js</t>
   </si>
@@ -1366,6 +1368,66 @@
   </si>
   <si>
     <t>router</t>
+  </si>
+  <si>
+    <t>starwars.vue</t>
+  </si>
+  <si>
+    <t>search</t>
+  </si>
+  <si>
+    <t>page-=1</t>
+  </si>
+  <si>
+    <t>page+=1</t>
+  </si>
+  <si>
+    <t>ul</t>
+  </si>
+  <si>
+    <t>v-for</t>
+  </si>
+  <si>
+    <t>items</t>
+  </si>
+  <si>
+    <t>button:Prev</t>
+  </si>
+  <si>
+    <t>button:Next</t>
+  </si>
+  <si>
+    <t>loadPlanets(){items = GET('https://techcrunch.com/wp-json' )}</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>ru</t>
+  </si>
+  <si>
+    <t>Поиск</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>en.json:</t>
+  </si>
+  <si>
+    <t>xxx.vue</t>
+  </si>
+  <si>
+    <t>Header.vue</t>
+  </si>
+  <si>
+    <t>search.vue</t>
+  </si>
+  <si>
+    <t>Selection_panel.vue</t>
+  </si>
+  <si>
+    <t>Choose_modification</t>
   </si>
 </sst>
 </file>
@@ -1600,7 +1662,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1704,10 +1766,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1716,22 +1796,10 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1745,6 +1813,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1776,15 +1856,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1793,6 +1868,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF00CCFF"/>
       <color rgb="FFFFFF99"/>
     </mruColors>
   </colors>
@@ -2584,8 +2660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A13F850-9F64-4DB4-B0B4-6110C995E04A}">
   <dimension ref="A1:BK262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="L100" sqref="L100"/>
+    <sheetView topLeftCell="A10" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -2606,42 +2682,42 @@
       <c r="D1" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="G1" s="93" t="s">
+      <c r="G1" s="103" t="s">
         <v>254</v>
       </c>
-      <c r="H1" s="94"/>
+      <c r="H1" s="104"/>
       <c r="I1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="93" t="s">
+      <c r="J1" s="103" t="s">
         <v>259</v>
       </c>
-      <c r="K1" s="94"/>
-      <c r="M1" s="93" t="s">
+      <c r="K1" s="104"/>
+      <c r="M1" s="103" t="s">
         <v>257</v>
       </c>
-      <c r="N1" s="94"/>
+      <c r="N1" s="104"/>
       <c r="O1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="93" t="s">
+      <c r="P1" s="103" t="s">
         <v>258</v>
       </c>
-      <c r="Q1" s="94"/>
+      <c r="Q1" s="104"/>
       <c r="R1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="93" t="s">
+      <c r="S1" s="103" t="s">
         <v>256</v>
       </c>
-      <c r="T1" s="94"/>
+      <c r="T1" s="104"/>
       <c r="U1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="V1" s="93" t="s">
+      <c r="V1" s="103" t="s">
         <v>260</v>
       </c>
-      <c r="W1" s="94"/>
+      <c r="W1" s="104"/>
       <c r="X1" s="15" t="s">
         <v>2</v>
       </c>
@@ -2707,10 +2783,10 @@
       <c r="R2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="S2" s="91" t="s">
+      <c r="S2" s="97" t="s">
         <v>193</v>
       </c>
-      <c r="T2" s="92"/>
+      <c r="T2" s="98"/>
       <c r="U2" s="15" t="s">
         <v>2</v>
       </c>
@@ -2746,24 +2822,24 @@
       <c r="B3" s="35" t="s">
         <v>159</v>
       </c>
-      <c r="G3" s="91" t="s">
+      <c r="G3" s="97" t="s">
         <v>255</v>
       </c>
-      <c r="H3" s="92"/>
+      <c r="H3" s="98"/>
       <c r="I3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="91" t="s">
+      <c r="J3" s="97" t="s">
         <v>158</v>
       </c>
-      <c r="K3" s="92"/>
+      <c r="K3" s="98"/>
       <c r="L3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="91" t="s">
+      <c r="M3" s="97" t="s">
         <v>258</v>
       </c>
-      <c r="N3" s="92"/>
+      <c r="N3" s="98"/>
       <c r="O3" s="15" t="s">
         <v>2</v>
       </c>
@@ -2836,17 +2912,17 @@
       <c r="O4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="P4" s="91" t="s">
+      <c r="P4" s="97" t="s">
         <v>188</v>
       </c>
-      <c r="Q4" s="92"/>
+      <c r="Q4" s="98"/>
       <c r="R4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="S4" s="91" t="s">
+      <c r="S4" s="97" t="s">
         <v>260</v>
       </c>
-      <c r="T4" s="92"/>
+      <c r="T4" s="98"/>
       <c r="U4" s="15" t="s">
         <v>2</v>
       </c>
@@ -2911,10 +2987,10 @@
       <c r="U5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="V5" s="91" t="s">
+      <c r="V5" s="97" t="s">
         <v>193</v>
       </c>
-      <c r="W5" s="92"/>
+      <c r="W5" s="98"/>
       <c r="X5" s="15" t="s">
         <v>2</v>
       </c>
@@ -3127,17 +3203,17 @@
       <c r="F12" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G12" s="99" t="s">
+      <c r="G12" s="107" t="s">
         <v>267</v>
       </c>
-      <c r="H12" s="100"/>
+      <c r="H12" s="108"/>
       <c r="I12" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="J12" s="93" t="s">
+      <c r="J12" s="103" t="s">
         <v>267</v>
       </c>
-      <c r="K12" s="94"/>
+      <c r="K12" s="104"/>
       <c r="L12" s="15" t="s">
         <v>2</v>
       </c>
@@ -3167,44 +3243,44 @@
       <c r="C13" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="89" t="s">
+      <c r="D13" s="101" t="s">
         <v>193</v>
       </c>
-      <c r="E13" s="90"/>
+      <c r="E13" s="102"/>
       <c r="F13" s="15" t="s">
         <v>2</v>
       </c>
       <c r="I13" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="J13" s="89" t="s">
+      <c r="J13" s="101" t="s">
         <v>227</v>
       </c>
-      <c r="K13" s="90"/>
+      <c r="K13" s="102"/>
       <c r="L13" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="M13" s="93" t="s">
+      <c r="M13" s="103" t="s">
         <v>270</v>
       </c>
-      <c r="N13" s="94"/>
+      <c r="N13" s="104"/>
       <c r="O13" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="P13" s="93" t="s">
+      <c r="P13" s="103" t="s">
         <v>162</v>
       </c>
-      <c r="Q13" s="94"/>
+      <c r="Q13" s="104"/>
       <c r="R13" s="15" t="s">
         <v>2</v>
       </c>
       <c r="X13" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Y13" s="93" t="s">
+      <c r="Y13" s="103" t="s">
         <v>298</v>
       </c>
-      <c r="Z13" s="94"/>
+      <c r="Z13" s="104"/>
       <c r="AD13" s="45" t="s">
         <v>2</v>
       </c>
@@ -3264,10 +3340,10 @@
       <c r="R14" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="S14" s="93" t="s">
+      <c r="S14" s="103" t="s">
         <v>179</v>
       </c>
-      <c r="T14" s="94"/>
+      <c r="T14" s="104"/>
       <c r="U14" s="15" t="s">
         <v>2</v>
       </c>
@@ -3283,10 +3359,10 @@
       <c r="AA14" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="AB14" s="93" t="s">
+      <c r="AB14" s="103" t="s">
         <v>301</v>
       </c>
-      <c r="AC14" s="94"/>
+      <c r="AC14" s="104"/>
       <c r="AD14" s="45" t="s">
         <v>2</v>
       </c>
@@ -3346,17 +3422,17 @@
       <c r="R15" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="S15" s="91" t="s">
+      <c r="S15" s="97" t="s">
         <v>164</v>
       </c>
-      <c r="T15" s="92"/>
+      <c r="T15" s="98"/>
       <c r="U15" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="V15" s="93" t="s">
+      <c r="V15" s="103" t="s">
         <v>195</v>
       </c>
-      <c r="W15" s="94"/>
+      <c r="W15" s="104"/>
       <c r="X15" s="15" t="s">
         <v>2</v>
       </c>
@@ -3378,10 +3454,10 @@
       <c r="AD15" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="AE15" s="93" t="s">
+      <c r="AE15" s="103" t="s">
         <v>310</v>
       </c>
-      <c r="AF15" s="94"/>
+      <c r="AF15" s="104"/>
       <c r="AG15" s="15" t="s">
         <v>2</v>
       </c>
@@ -3390,10 +3466,10 @@
       </c>
     </row>
     <row r="16" spans="1:63" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="87" t="s">
+      <c r="A16" s="109" t="s">
         <v>392</v>
       </c>
-      <c r="B16" s="88"/>
+      <c r="B16" s="110"/>
       <c r="C16" s="15" t="s">
         <v>2</v>
       </c>
@@ -3409,24 +3485,24 @@
       <c r="I16" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="J16" s="89" t="s">
+      <c r="J16" s="101" t="s">
         <v>280</v>
       </c>
-      <c r="K16" s="90"/>
+      <c r="K16" s="102"/>
       <c r="L16" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="M16" s="91" t="s">
+      <c r="M16" s="97" t="s">
         <v>164</v>
       </c>
-      <c r="N16" s="92"/>
+      <c r="N16" s="98"/>
       <c r="O16" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="P16" s="89" t="s">
+      <c r="P16" s="101" t="s">
         <v>193</v>
       </c>
-      <c r="Q16" s="90"/>
+      <c r="Q16" s="102"/>
       <c r="R16" s="15" t="s">
         <v>2</v>
       </c>
@@ -3448,17 +3524,17 @@
       <c r="X16" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Y16" s="89" t="s">
+      <c r="Y16" s="101" t="s">
         <v>193</v>
       </c>
-      <c r="Z16" s="90"/>
+      <c r="Z16" s="102"/>
       <c r="AA16" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="AB16" s="91" t="s">
+      <c r="AB16" s="97" t="s">
         <v>164</v>
       </c>
-      <c r="AC16" s="92"/>
+      <c r="AC16" s="98"/>
       <c r="AD16" s="45" t="s">
         <v>2</v>
       </c>
@@ -3471,10 +3547,10 @@
       <c r="AG16" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="AH16" s="93" t="s">
+      <c r="AH16" s="103" t="s">
         <v>335</v>
       </c>
-      <c r="AI16" s="94"/>
+      <c r="AI16" s="104"/>
       <c r="AJ16" s="15" t="s">
         <v>2</v>
       </c>
@@ -3564,10 +3640,10 @@
       <c r="AD17" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="AE17" s="91" t="s">
+      <c r="AE17" s="97" t="s">
         <v>423</v>
       </c>
-      <c r="AF17" s="92"/>
+      <c r="AF17" s="98"/>
       <c r="AG17" s="15" t="s">
         <v>2</v>
       </c>
@@ -3580,10 +3656,10 @@
       <c r="AJ17" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="AK17" s="93" t="s">
+      <c r="AK17" s="103" t="s">
         <v>164</v>
       </c>
-      <c r="AL17" s="94"/>
+      <c r="AL17" s="104"/>
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A18" s="83" t="s">
@@ -3643,11 +3719,11 @@
       <c r="U18" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="V18" s="91" t="str">
+      <c r="V18" s="97" t="str">
         <f>components!A2</f>
         <v>Dialog/DialogF.vue</v>
       </c>
-      <c r="W18" s="92"/>
+      <c r="W18" s="98"/>
       <c r="X18" s="15" t="s">
         <v>2</v>
       </c>
@@ -3788,10 +3864,10 @@
       <c r="AG19" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="AH19" s="91" t="s">
+      <c r="AH19" s="97" t="s">
         <v>164</v>
       </c>
-      <c r="AI19" s="92"/>
+      <c r="AI19" s="98"/>
       <c r="AJ19" s="15" t="s">
         <v>2</v>
       </c>
@@ -3812,20 +3888,20 @@
       <c r="C20" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="99" t="s">
+      <c r="D20" s="107" t="s">
         <v>441</v>
       </c>
-      <c r="E20" s="100"/>
+      <c r="E20" s="108"/>
       <c r="F20" s="15" t="s">
         <v>2</v>
       </c>
       <c r="I20" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="J20" s="89" t="s">
+      <c r="J20" s="101" t="s">
         <v>281</v>
       </c>
-      <c r="K20" s="90"/>
+      <c r="K20" s="102"/>
       <c r="L20" s="15" t="s">
         <v>2</v>
       </c>
@@ -3847,10 +3923,10 @@
       <c r="R20" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="S20" s="91" t="s">
+      <c r="S20" s="97" t="s">
         <v>188</v>
       </c>
-      <c r="T20" s="92"/>
+      <c r="T20" s="98"/>
       <c r="U20" s="15" t="s">
         <v>2</v>
       </c>
@@ -3893,16 +3969,16 @@
       <c r="AJ20" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="AK20" s="91" t="s">
+      <c r="AK20" s="97" t="s">
         <v>171</v>
       </c>
-      <c r="AL20" s="92"/>
+      <c r="AL20" s="98"/>
     </row>
     <row r="21" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="87" t="s">
+      <c r="A21" s="109" t="s">
         <v>393</v>
       </c>
-      <c r="B21" s="88"/>
+      <c r="B21" s="110"/>
       <c r="C21" s="15" t="s">
         <v>2</v>
       </c>
@@ -3921,10 +3997,10 @@
       <c r="L21" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="M21" s="89" t="s">
+      <c r="M21" s="101" t="s">
         <v>227</v>
       </c>
-      <c r="N21" s="90"/>
+      <c r="N21" s="102"/>
       <c r="O21" s="15" t="s">
         <v>2</v>
       </c>
@@ -3951,10 +4027,10 @@
       <c r="X21" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Y21" s="95" t="s">
+      <c r="Y21" s="99" t="s">
         <v>240</v>
       </c>
-      <c r="Z21" s="96"/>
+      <c r="Z21" s="100"/>
       <c r="AA21" s="15" t="s">
         <v>2</v>
       </c>
@@ -4008,10 +4084,10 @@
       <c r="I22" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="J22" s="89" t="s">
+      <c r="J22" s="101" t="s">
         <v>282</v>
       </c>
-      <c r="K22" s="90"/>
+      <c r="K22" s="102"/>
       <c r="L22" s="15" t="s">
         <v>2</v>
       </c>
@@ -4024,10 +4100,10 @@
       <c r="O22" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="P22" s="95" t="s">
+      <c r="P22" s="99" t="s">
         <v>240</v>
       </c>
-      <c r="Q22" s="96"/>
+      <c r="Q22" s="100"/>
       <c r="R22" s="15" t="s">
         <v>2</v>
       </c>
@@ -4135,31 +4211,31 @@
       <c r="R23" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="S23" s="91" t="s">
+      <c r="S23" s="97" t="s">
         <v>423</v>
       </c>
-      <c r="T23" s="92"/>
+      <c r="T23" s="98"/>
       <c r="U23" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="V23" s="89" t="s">
+      <c r="V23" s="101" t="s">
         <v>227</v>
       </c>
-      <c r="W23" s="90"/>
+      <c r="W23" s="102"/>
       <c r="X23" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Y23" s="97" t="s">
+      <c r="Y23" s="105" t="s">
         <v>301</v>
       </c>
-      <c r="Z23" s="98"/>
+      <c r="Z23" s="106"/>
       <c r="AA23" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="AB23" s="91" t="s">
+      <c r="AB23" s="97" t="s">
         <v>310</v>
       </c>
-      <c r="AC23" s="92"/>
+      <c r="AC23" s="98"/>
       <c r="AD23" s="45" t="s">
         <v>2</v>
       </c>
@@ -4198,24 +4274,24 @@
       <c r="I24" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="J24" s="89" t="s">
+      <c r="J24" s="101" t="s">
         <v>283</v>
       </c>
-      <c r="K24" s="90"/>
+      <c r="K24" s="102"/>
       <c r="L24" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="M24" s="89" t="s">
+      <c r="M24" s="101" t="s">
         <v>273</v>
       </c>
-      <c r="N24" s="90"/>
+      <c r="N24" s="102"/>
       <c r="O24" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="P24" s="97" t="s">
+      <c r="P24" s="105" t="s">
         <v>179</v>
       </c>
-      <c r="Q24" s="98"/>
+      <c r="Q24" s="106"/>
       <c r="R24" s="15" t="s">
         <v>2</v>
       </c>
@@ -4356,19 +4432,19 @@
       <c r="AG25" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="AH25" s="89" t="s">
+      <c r="AH25" s="101" t="s">
         <v>227</v>
       </c>
-      <c r="AI25" s="90"/>
+      <c r="AI25" s="102"/>
       <c r="AJ25" s="15" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="87" t="s">
+      <c r="A26" s="109" t="s">
         <v>397</v>
       </c>
-      <c r="B26" s="88"/>
+      <c r="B26" s="110"/>
       <c r="C26" s="15" t="s">
         <v>2</v>
       </c>
@@ -4378,17 +4454,17 @@
       <c r="I26" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="J26" s="91" t="s">
+      <c r="J26" s="97" t="s">
         <v>162</v>
       </c>
-      <c r="K26" s="92"/>
+      <c r="K26" s="98"/>
       <c r="L26" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="M26" s="89" t="s">
+      <c r="M26" s="101" t="s">
         <v>278</v>
       </c>
-      <c r="N26" s="90"/>
+      <c r="N26" s="102"/>
       <c r="O26" s="15" t="s">
         <v>2</v>
       </c>
@@ -4410,10 +4486,10 @@
       <c r="U26" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="V26" s="89" t="s">
+      <c r="V26" s="101" t="s">
         <v>228</v>
       </c>
-      <c r="W26" s="90"/>
+      <c r="W26" s="102"/>
       <c r="X26" s="15" t="s">
         <v>2</v>
       </c>
@@ -4429,10 +4505,10 @@
       <c r="AD26" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="AE26" s="95" t="s">
+      <c r="AE26" s="99" t="s">
         <v>240</v>
       </c>
-      <c r="AF26" s="96"/>
+      <c r="AF26" s="100"/>
       <c r="AG26" s="15" t="s">
         <v>2</v>
       </c>
@@ -4504,10 +4580,10 @@
       <c r="AA27" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="AB27" s="91" t="s">
+      <c r="AB27" s="97" t="s">
         <v>310</v>
       </c>
-      <c r="AC27" s="92"/>
+      <c r="AC27" s="98"/>
       <c r="AD27" s="45" t="s">
         <v>2</v>
       </c>
@@ -4546,17 +4622,17 @@
       <c r="I28" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="J28" s="91" t="s">
+      <c r="J28" s="97" t="s">
         <v>298</v>
       </c>
-      <c r="K28" s="92"/>
+      <c r="K28" s="98"/>
       <c r="L28" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="M28" s="89" t="s">
+      <c r="M28" s="101" t="s">
         <v>279</v>
       </c>
-      <c r="N28" s="90"/>
+      <c r="N28" s="102"/>
       <c r="O28" s="15" t="s">
         <v>2</v>
       </c>
@@ -4593,17 +4669,17 @@
       <c r="AD28" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="AE28" s="91" t="s">
+      <c r="AE28" s="97" t="s">
         <v>335</v>
       </c>
-      <c r="AF28" s="92"/>
+      <c r="AF28" s="98"/>
       <c r="AG28" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="AH28" s="89" t="s">
+      <c r="AH28" s="101" t="s">
         <v>332</v>
       </c>
-      <c r="AI28" s="90"/>
+      <c r="AI28" s="102"/>
       <c r="AJ28" s="15" t="s">
         <v>2</v>
       </c>
@@ -4654,10 +4730,10 @@
       <c r="U29" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="V29" s="89" t="s">
+      <c r="V29" s="101" t="s">
         <v>229</v>
       </c>
-      <c r="W29" s="90"/>
+      <c r="W29" s="102"/>
       <c r="X29" s="15" t="s">
         <v>2</v>
       </c>
@@ -4708,10 +4784,10 @@
       <c r="I30" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="J30" s="99" t="s">
+      <c r="J30" s="107" t="s">
         <v>163</v>
       </c>
-      <c r="K30" s="100"/>
+      <c r="K30" s="108"/>
       <c r="L30" s="15" t="s">
         <v>2</v>
       </c>
@@ -4760,10 +4836,10 @@
       <c r="AG30" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="AH30" s="91" t="s">
+      <c r="AH30" s="97" t="s">
         <v>333</v>
       </c>
-      <c r="AI30" s="92"/>
+      <c r="AI30" s="98"/>
       <c r="AJ30" s="15" t="s">
         <v>2</v>
       </c>
@@ -4790,20 +4866,20 @@
       <c r="U31" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="V31" s="89" t="s">
+      <c r="V31" s="101" t="s">
         <v>230</v>
       </c>
-      <c r="W31" s="90"/>
+      <c r="W31" s="102"/>
       <c r="X31" s="15" t="s">
         <v>2</v>
       </c>
       <c r="AA31" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="AB31" s="91" t="s">
+      <c r="AB31" s="97" t="s">
         <v>310</v>
       </c>
-      <c r="AC31" s="92"/>
+      <c r="AC31" s="98"/>
       <c r="AD31" s="45" t="s">
         <v>2</v>
       </c>
@@ -4830,10 +4906,10 @@
       <c r="I32" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="J32" s="95" t="s">
+      <c r="J32" s="99" t="s">
         <v>240</v>
       </c>
-      <c r="K32" s="96"/>
+      <c r="K32" s="100"/>
       <c r="L32" s="15" t="s">
         <v>2</v>
       </c>
@@ -4843,10 +4919,10 @@
       <c r="R32" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="S32" s="95" t="s">
+      <c r="S32" s="99" t="s">
         <v>240</v>
       </c>
-      <c r="T32" s="96"/>
+      <c r="T32" s="100"/>
       <c r="U32" s="15" t="s">
         <v>2</v>
       </c>
@@ -4944,10 +5020,10 @@
       <c r="I34" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="J34" s="91" t="s">
+      <c r="J34" s="97" t="s">
         <v>271</v>
       </c>
-      <c r="K34" s="92"/>
+      <c r="K34" s="98"/>
       <c r="L34" s="15" t="s">
         <v>2</v>
       </c>
@@ -4957,11 +5033,11 @@
       <c r="R34" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="S34" s="91" t="str">
+      <c r="S34" s="97" t="str">
         <f>V15</f>
         <v>Dialog/NotificationDialog.vue</v>
       </c>
-      <c r="T34" s="92"/>
+      <c r="T34" s="98"/>
       <c r="U34" s="15" t="s">
         <v>2</v>
       </c>
@@ -5021,10 +5097,10 @@
       <c r="AA35" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="AB35" s="91" t="s">
+      <c r="AB35" s="97" t="s">
         <v>310</v>
       </c>
-      <c r="AC35" s="92"/>
+      <c r="AC35" s="98"/>
       <c r="AD35" s="45" t="s">
         <v>2</v>
       </c>
@@ -5211,10 +5287,10 @@
       <c r="C42" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="89" t="s">
+      <c r="D42" s="101" t="s">
         <v>193</v>
       </c>
-      <c r="E42" s="90"/>
+      <c r="E42" s="102"/>
       <c r="F42" s="15" t="s">
         <v>2</v>
       </c>
@@ -5313,10 +5389,10 @@
       </c>
     </row>
     <row r="46" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A46" s="87" t="s">
+      <c r="A46" s="109" t="s">
         <v>392</v>
       </c>
-      <c r="B46" s="88"/>
+      <c r="B46" s="110"/>
       <c r="C46" s="15" t="s">
         <v>2</v>
       </c>
@@ -5420,10 +5496,10 @@
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A51" s="87" t="s">
+      <c r="A51" s="109" t="s">
         <v>393</v>
       </c>
-      <c r="B51" s="88"/>
+      <c r="B51" s="110"/>
       <c r="C51" s="15" t="s">
         <v>2</v>
       </c>
@@ -5488,10 +5564,10 @@
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A56" s="87" t="s">
+      <c r="A56" s="109" t="s">
         <v>397</v>
       </c>
-      <c r="B56" s="88"/>
+      <c r="B56" s="110"/>
       <c r="C56" s="15" t="s">
         <v>2</v>
       </c>
@@ -5645,17 +5721,17 @@
       <c r="C66" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D66" s="91" t="s">
+      <c r="D66" s="97" t="s">
         <v>423</v>
       </c>
-      <c r="E66" s="92"/>
+      <c r="E66" s="98"/>
       <c r="F66" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G66" s="89" t="s">
+      <c r="G66" s="101" t="s">
         <v>227</v>
       </c>
-      <c r="H66" s="90"/>
+      <c r="H66" s="102"/>
       <c r="I66" s="15" t="s">
         <v>2</v>
       </c>
@@ -5670,10 +5746,10 @@
       <c r="C67" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D67" s="89" t="s">
+      <c r="D67" s="101" t="s">
         <v>193</v>
       </c>
-      <c r="E67" s="90"/>
+      <c r="E67" s="102"/>
       <c r="F67" s="15" t="s">
         <v>2</v>
       </c>
@@ -5717,10 +5793,10 @@
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A69" s="87" t="s">
+      <c r="A69" s="109" t="s">
         <v>392</v>
       </c>
-      <c r="B69" s="88"/>
+      <c r="B69" s="110"/>
       <c r="C69" s="15" t="s">
         <v>2</v>
       </c>
@@ -5733,10 +5809,10 @@
       <c r="F69" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G69" s="89" t="s">
+      <c r="G69" s="101" t="s">
         <v>273</v>
       </c>
-      <c r="H69" s="90"/>
+      <c r="H69" s="102"/>
       <c r="I69" s="15" t="s">
         <v>2</v>
       </c>
@@ -5840,10 +5916,10 @@
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A74" s="87" t="s">
+      <c r="A74" s="109" t="s">
         <v>393</v>
       </c>
-      <c r="B74" s="88"/>
+      <c r="B74" s="110"/>
       <c r="C74" s="15" t="s">
         <v>2</v>
       </c>
@@ -5947,10 +6023,10 @@
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79" s="87" t="s">
+      <c r="A79" s="109" t="s">
         <v>397</v>
       </c>
-      <c r="B79" s="88"/>
+      <c r="B79" s="110"/>
       <c r="C79" s="15" t="s">
         <v>2</v>
       </c>
@@ -6063,19 +6139,19 @@
       </c>
     </row>
     <row r="94" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="111"/>
-      <c r="B94" s="112" t="s">
+      <c r="A94" s="87"/>
+      <c r="B94" s="111" t="s">
         <v>445</v>
       </c>
-      <c r="C94" s="112"/>
-      <c r="D94" s="112" t="s">
+      <c r="C94" s="111"/>
+      <c r="D94" s="111" t="s">
         <v>157</v>
       </c>
-      <c r="E94" s="112"/>
-      <c r="F94" s="112" t="s">
+      <c r="E94" s="111"/>
+      <c r="F94" s="111" t="s">
         <v>370</v>
       </c>
-      <c r="G94" s="113"/>
+      <c r="G94" s="112"/>
       <c r="I94" s="15" t="s">
         <v>2</v>
       </c>
@@ -6102,7 +6178,7 @@
       <c r="A96" s="83" t="s">
         <v>442</v>
       </c>
-      <c r="B96" s="115" t="s">
+      <c r="B96" s="89" t="s">
         <v>425</v>
       </c>
       <c r="C96" s="62" t="s">
@@ -6142,7 +6218,7 @@
       <c r="A98" s="85" t="s">
         <v>444</v>
       </c>
-      <c r="B98" s="114" t="s">
+      <c r="B98" s="88" t="s">
         <v>383</v>
       </c>
       <c r="C98" s="14" t="s">
@@ -7009,11 +7085,31 @@
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="B94:C94"/>
     <mergeCell ref="D94:E94"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A56:B56"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="F94:G94"/>
     <mergeCell ref="AK20:AL20"/>
     <mergeCell ref="AK17:AL17"/>
+    <mergeCell ref="AE15:AF15"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="S34:T34"/>
+    <mergeCell ref="V15:W15"/>
+    <mergeCell ref="V18:W18"/>
+    <mergeCell ref="V26:W26"/>
+    <mergeCell ref="V29:W29"/>
+    <mergeCell ref="V31:W31"/>
+    <mergeCell ref="Y13:Z13"/>
+    <mergeCell ref="J24:K24"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="V5:W5"/>
     <mergeCell ref="G1:H1"/>
@@ -7027,15 +7123,6 @@
     <mergeCell ref="S1:T1"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="S4:T4"/>
-    <mergeCell ref="AE15:AF15"/>
-    <mergeCell ref="S23:T23"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="S34:T34"/>
-    <mergeCell ref="V15:W15"/>
-    <mergeCell ref="V18:W18"/>
-    <mergeCell ref="V26:W26"/>
-    <mergeCell ref="V29:W29"/>
-    <mergeCell ref="V31:W31"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="J32:K32"/>
     <mergeCell ref="J34:K34"/>
@@ -7049,11 +7136,9 @@
     <mergeCell ref="J12:K12"/>
     <mergeCell ref="J22:K22"/>
     <mergeCell ref="J13:K13"/>
-    <mergeCell ref="Y13:Z13"/>
     <mergeCell ref="J28:K28"/>
     <mergeCell ref="J16:K16"/>
     <mergeCell ref="M13:N13"/>
-    <mergeCell ref="J24:K24"/>
     <mergeCell ref="J26:K26"/>
     <mergeCell ref="P13:Q13"/>
     <mergeCell ref="P22:Q22"/>
@@ -7077,20 +7162,11 @@
     <mergeCell ref="AH25:AI25"/>
     <mergeCell ref="AH28:AI28"/>
     <mergeCell ref="AE17:AF17"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="A69:B69"/>
     <mergeCell ref="AB31:AC31"/>
     <mergeCell ref="AB35:AC35"/>
     <mergeCell ref="S32:T32"/>
     <mergeCell ref="G66:H66"/>
     <mergeCell ref="G69:H69"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A56:B56"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="50" orientation="landscape" r:id="rId1"/>
@@ -7117,33 +7193,33 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="103" t="s">
         <v>164</v>
       </c>
-      <c r="B2" s="94"/>
+      <c r="B2" s="104"/>
       <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="93" t="s">
+      <c r="D2" s="103" t="s">
         <v>423</v>
       </c>
-      <c r="E2" s="94"/>
+      <c r="E2" s="104"/>
       <c r="F2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="91" t="s">
+      <c r="A3" s="97" t="s">
         <v>171</v>
       </c>
-      <c r="B3" s="92"/>
+      <c r="B3" s="98"/>
       <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="91" t="s">
+      <c r="D3" s="97" t="s">
         <v>199</v>
       </c>
-      <c r="E3" s="92"/>
+      <c r="E3" s="98"/>
       <c r="F3" t="s">
         <v>2</v>
       </c>
@@ -7229,26 +7305,26 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="101" t="s">
+      <c r="A8" s="113" t="s">
         <v>174</v>
       </c>
-      <c r="B8" s="102"/>
+      <c r="B8" s="114"/>
       <c r="C8" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="91" t="s">
+      <c r="D8" s="97" t="s">
         <v>207</v>
       </c>
-      <c r="E8" s="92"/>
+      <c r="E8" s="98"/>
       <c r="F8" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="91" t="s">
+      <c r="A9" s="97" t="s">
         <v>172</v>
       </c>
-      <c r="B9" s="92"/>
+      <c r="B9" s="98"/>
       <c r="C9" t="s">
         <v>2</v>
       </c>
@@ -7272,19 +7348,19 @@
       <c r="C10" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="91" t="s">
+      <c r="D10" s="97" t="s">
         <v>209</v>
       </c>
-      <c r="E10" s="92"/>
+      <c r="E10" s="98"/>
       <c r="F10" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="91" t="s">
+      <c r="A11" s="97" t="s">
         <v>172</v>
       </c>
-      <c r="B11" s="92"/>
+      <c r="B11" s="98"/>
       <c r="C11" t="s">
         <v>2</v>
       </c>
@@ -7330,28 +7406,28 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D14" s="89" t="s">
+      <c r="D14" s="101" t="s">
         <v>215</v>
       </c>
-      <c r="E14" s="90"/>
+      <c r="E14" s="102"/>
       <c r="F14" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D15" s="89" t="s">
+      <c r="D15" s="101" t="s">
         <v>216</v>
       </c>
-      <c r="E15" s="90"/>
+      <c r="E15" s="102"/>
       <c r="F15" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D16" s="89" t="s">
+      <c r="D16" s="101" t="s">
         <v>221</v>
       </c>
-      <c r="E16" s="90"/>
+      <c r="E16" s="102"/>
       <c r="F16" t="s">
         <v>2</v>
       </c>
@@ -7532,7 +7608,7 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A2" s="103" t="s">
+      <c r="A2" s="115" t="s">
         <v>88</v>
       </c>
       <c r="B2" s="1"/>
@@ -7564,7 +7640,7 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A3" s="103"/>
+      <c r="A3" s="115"/>
       <c r="B3" s="1"/>
       <c r="D3" s="1" t="s">
         <v>18</v>
@@ -7613,7 +7689,7 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="104"/>
+      <c r="A4" s="116"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
@@ -7640,7 +7716,7 @@
       <c r="O4" s="2"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A5" s="105" t="s">
+      <c r="A5" s="117" t="s">
         <v>89</v>
       </c>
       <c r="B5" s="5"/>
@@ -7668,7 +7744,7 @@
       <c r="O5" s="5"/>
     </row>
     <row r="6" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="104"/>
+      <c r="A6" s="116"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
@@ -7695,7 +7771,7 @@
       <c r="O6" s="2"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A7" s="106" t="s">
+      <c r="A7" s="118" t="s">
         <v>90</v>
       </c>
       <c r="B7" s="5"/>
@@ -7727,7 +7803,7 @@
       <c r="O7" s="5"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A8" s="107"/>
+      <c r="A8" s="119"/>
       <c r="B8" s="1"/>
       <c r="D8" s="22" t="s">
         <v>30</v>
@@ -7755,7 +7831,7 @@
       <c r="O8" s="1"/>
     </row>
     <row r="9" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="108"/>
+      <c r="A9" s="120"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="19" t="s">
@@ -7784,7 +7860,7 @@
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A10" s="105" t="s">
+      <c r="A10" s="117" t="s">
         <v>94</v>
       </c>
       <c r="B10" s="5"/>
@@ -7830,7 +7906,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="104"/>
+      <c r="A11" s="116"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="19" t="s">
@@ -7857,7 +7933,7 @@
       <c r="O11" s="11"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A12" s="103" t="s">
+      <c r="A12" s="115" t="s">
         <v>95</v>
       </c>
       <c r="B12" s="1"/>
@@ -7889,7 +7965,7 @@
       <c r="O12" s="12"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A13" s="103"/>
+      <c r="A13" s="115"/>
       <c r="B13" s="1"/>
       <c r="D13" s="1" t="s">
         <v>27</v>
@@ -7909,7 +7985,7 @@
       <c r="O13" s="12"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A14" s="103"/>
+      <c r="A14" s="115"/>
       <c r="B14" s="1"/>
       <c r="D14" s="1" t="s">
         <v>26</v>
@@ -7929,7 +8005,7 @@
       <c r="O14" s="12"/>
     </row>
     <row r="15" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="104"/>
+      <c r="A15" s="116"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
@@ -7983,10 +8059,10 @@
       <c r="O16" s="12"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A17" s="105" t="s">
+      <c r="A17" s="117" t="s">
         <v>112</v>
       </c>
-      <c r="B17" s="109" t="s">
+      <c r="B17" s="121" t="s">
         <v>133</v>
       </c>
       <c r="C17" s="5"/>
@@ -8008,8 +8084,8 @@
       <c r="O17" s="5"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A18" s="103"/>
-      <c r="B18" s="110"/>
+      <c r="A18" s="115"/>
+      <c r="B18" s="122"/>
       <c r="C18" s="1"/>
       <c r="D18" s="3" t="s">
         <v>13</v>
@@ -8029,8 +8105,8 @@
       <c r="O18" s="1"/>
     </row>
     <row r="19" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="103"/>
-      <c r="B19" s="104"/>
+      <c r="A19" s="115"/>
+      <c r="B19" s="116"/>
       <c r="C19" s="2"/>
       <c r="D19" s="18" t="s">
         <v>14</v>
@@ -8050,8 +8126,8 @@
       <c r="O19" s="2"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A20" s="103"/>
-      <c r="B20" s="105" t="s">
+      <c r="A20" s="115"/>
+      <c r="B20" s="117" t="s">
         <v>10</v>
       </c>
       <c r="C20" s="5"/>
@@ -8073,8 +8149,8 @@
       <c r="O20" s="5"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A21" s="103"/>
-      <c r="B21" s="103"/>
+      <c r="A21" s="115"/>
+      <c r="B21" s="115"/>
       <c r="C21" s="1"/>
       <c r="D21" s="3" t="s">
         <v>129</v>
@@ -8094,8 +8170,8 @@
       <c r="O21" s="1"/>
     </row>
     <row r="22" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="103"/>
-      <c r="B22" s="104"/>
+      <c r="A22" s="115"/>
+      <c r="B22" s="116"/>
       <c r="C22" s="2"/>
       <c r="D22" s="18" t="s">
         <v>130</v>
@@ -8115,8 +8191,8 @@
       <c r="O22" s="2"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A23" s="103"/>
-      <c r="B23" s="105" t="s">
+      <c r="A23" s="115"/>
+      <c r="B23" s="117" t="s">
         <v>3</v>
       </c>
       <c r="C23" s="5"/>
@@ -8138,8 +8214,8 @@
       <c r="O23" s="5"/>
     </row>
     <row r="24" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="103"/>
-      <c r="B24" s="104"/>
+      <c r="A24" s="115"/>
+      <c r="B24" s="116"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
         <v>0</v>
@@ -8171,8 +8247,8 @@
       <c r="O24" s="2"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A25" s="103"/>
-      <c r="B25" s="105" t="s">
+      <c r="A25" s="115"/>
+      <c r="B25" s="117" t="s">
         <v>11</v>
       </c>
       <c r="C25" s="5"/>
@@ -8194,8 +8270,8 @@
       <c r="O25" s="5"/>
     </row>
     <row r="26" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="103"/>
-      <c r="B26" s="104"/>
+      <c r="A26" s="115"/>
+      <c r="B26" s="116"/>
       <c r="C26" s="2"/>
       <c r="D26" s="18" t="s">
         <v>126</v>
@@ -8215,7 +8291,7 @@
       <c r="O26" s="2"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A27" s="103"/>
+      <c r="A27" s="115"/>
       <c r="B27" s="1" t="s">
         <v>35</v>
       </c>
@@ -8250,7 +8326,7 @@
       <c r="O27" s="1"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A28" s="103"/>
+      <c r="A28" s="115"/>
       <c r="B28" s="1" t="s">
         <v>35</v>
       </c>
@@ -8285,7 +8361,7 @@
       <c r="O28" s="1"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A29" s="103"/>
+      <c r="A29" s="115"/>
       <c r="B29" s="3" t="s">
         <v>35</v>
       </c>
@@ -8306,7 +8382,7 @@
       <c r="O29" s="1"/>
     </row>
     <row r="30" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="104"/>
+      <c r="A30" s="116"/>
       <c r="B30" s="18" t="s">
         <v>35</v>
       </c>
@@ -8327,7 +8403,7 @@
       <c r="O30" s="2"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A31" s="103" t="s">
+      <c r="A31" s="115" t="s">
         <v>137</v>
       </c>
       <c r="B31" s="1"/>
@@ -8347,7 +8423,7 @@
       <c r="O31" s="1"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A32" s="103"/>
+      <c r="A32" s="115"/>
       <c r="B32" s="1"/>
       <c r="D32" s="1" t="s">
         <v>24</v>
@@ -8367,7 +8443,7 @@
       <c r="O32" s="1"/>
     </row>
     <row r="33" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="103"/>
+      <c r="A33" s="115"/>
       <c r="B33" s="1"/>
       <c r="C33" s="2"/>
       <c r="D33" s="1" t="s">
@@ -8388,7 +8464,7 @@
       <c r="O33" s="1"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A34" s="105" t="s">
+      <c r="A34" s="117" t="s">
         <v>138</v>
       </c>
       <c r="B34" s="5"/>
@@ -8410,7 +8486,7 @@
       <c r="O34" s="5"/>
     </row>
     <row r="35" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="104"/>
+      <c r="A35" s="116"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
@@ -8592,4 +8668,1004 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23611E25-25E0-4416-94BB-E061D06323D6}">
+  <dimension ref="A1:D172"/>
+  <sheetViews>
+    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="90" t="s">
+        <v>446</v>
+      </c>
+      <c r="B2" s="62"/>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="94" t="s">
+        <v>420</v>
+      </c>
+      <c r="B3" s="95" t="s">
+        <v>455</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="91" t="s">
+        <v>158</v>
+      </c>
+      <c r="B4" s="92" t="s">
+        <v>447</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="96" t="s">
+        <v>453</v>
+      </c>
+      <c r="B5" s="96" t="s">
+        <v>448</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="96" t="s">
+        <v>454</v>
+      </c>
+      <c r="B6" s="96" t="s">
+        <v>449</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="123" t="s">
+        <v>450</v>
+      </c>
+      <c r="B7" s="123"/>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="92" t="s">
+        <v>451</v>
+      </c>
+      <c r="B8" s="92" t="s">
+        <v>452</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="93" t="s">
+        <v>225</v>
+      </c>
+      <c r="B9" s="93" t="s">
+        <v>376</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C29" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C33" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C35" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C36" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C37" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C41" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C42" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C43" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C44" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C45" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C46" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C47" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C48" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C49" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C50" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C51" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C52" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C53" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C54" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C55" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C56" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C57" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C58" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C59" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C60" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C61" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C62" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C63" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C64" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C65" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C66" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C67" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C68" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C69" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C70" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C71" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C72" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C73" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C74" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C75" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C76" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C77" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C78" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C79" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C80" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C81" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C82" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C83" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C84" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C85" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C86" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C87" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C88" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C89" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C90" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C91" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C92" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C93" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C94" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C95" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C96" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C97" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C98" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C99" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C100" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C101" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C102" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C103" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C104" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C105" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C106" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C107" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C108" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C109" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C110" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C111" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C112" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C113" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C114" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C115" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C116" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C117" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C118" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C119" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C120" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C121" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C122" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C123" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C124" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C125" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C126" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C127" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C128" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C129" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C130" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C131" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C132" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C133" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C134" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C135" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C136" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C137" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C138" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="139" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C139" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C140" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C141" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C142" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C143" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C144" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="145" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C145" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C146" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C147" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C148" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C149" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C150" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="151" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C151" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C152" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="153" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C153" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="154" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C154" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C155" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="156" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C156" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="157" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C157" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="158" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C158" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="159" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C159" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="160" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C160" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="161" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C161" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="162" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C162" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="163" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C163" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C164" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="165" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C165" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="166" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C166" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="167" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C167" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="168" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C168" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="169" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C169" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C170" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="171" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C171" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="172" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C172" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A7:B7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B182AE4-6249-418E-BEE5-6F13E9835A4F}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>456</v>
+      </c>
+      <c r="B1" t="s">
+        <v>457</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="124" t="s">
+        <v>459</v>
+      </c>
+      <c r="B2" s="124" t="s">
+        <v>458</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>463</v>
+      </c>
+      <c r="F2" t="s">
+        <v>464</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>460</v>
+      </c>
+      <c r="B3" t="str">
+        <f>A2</f>
+        <v>Search</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>461</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>